<commit_message>
1. Added Navigation drawer 2. Added MBA papers
</commit_message>
<xml_diff>
--- a/Nomenclature/Nomenclature.xlsx
+++ b/Nomenclature/Nomenclature.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raghav aggarwal\Downloads\KurukshetraUniversitypapers\Nomenclature\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raghav aggarwal\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="406">
   <si>
     <t>Country</t>
   </si>
@@ -876,6 +876,348 @@
     <t xml:space="preserve">Communication system </t>
   </si>
   <si>
+    <t>Fundamentals of microprocessor interfacing and application</t>
+  </si>
+  <si>
+    <t>FR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fundamentals of entrepreneurship </t>
+  </si>
+  <si>
+    <t>FE</t>
+  </si>
+  <si>
+    <t>Advance database system</t>
+  </si>
+  <si>
+    <t>AV</t>
+  </si>
+  <si>
+    <t>Information security</t>
+  </si>
+  <si>
+    <t>IS</t>
+  </si>
+  <si>
+    <t>Management</t>
+  </si>
+  <si>
+    <t>BBA</t>
+  </si>
+  <si>
+    <t>Business accounting</t>
+  </si>
+  <si>
+    <t>Managerial economics</t>
+  </si>
+  <si>
+    <t>Business mathematics</t>
+  </si>
+  <si>
+    <t>Hindi</t>
+  </si>
+  <si>
+    <t>Computer fundamentals</t>
+  </si>
+  <si>
+    <t>BA</t>
+  </si>
+  <si>
+    <t>BM</t>
+  </si>
+  <si>
+    <t>CF</t>
+  </si>
+  <si>
+    <t>MN</t>
+  </si>
+  <si>
+    <t>BS</t>
+  </si>
+  <si>
+    <t>HI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Understanding human behaviour </t>
+  </si>
+  <si>
+    <t>Micro business environment</t>
+  </si>
+  <si>
+    <t>Business statistics</t>
+  </si>
+  <si>
+    <t>UH</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>Managenent accounting</t>
+  </si>
+  <si>
+    <t>Fundamnetals of DBMS and ORACLE</t>
+  </si>
+  <si>
+    <t>Principles of management</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Understanding social behaviour </t>
+  </si>
+  <si>
+    <t>Business communication</t>
+  </si>
+  <si>
+    <t>BU</t>
+  </si>
+  <si>
+    <t>MG</t>
+  </si>
+  <si>
+    <t>FD</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>MBA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Business research methodology </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Financial management </t>
+  </si>
+  <si>
+    <t>Human resource management</t>
+  </si>
+  <si>
+    <t>Management science</t>
+  </si>
+  <si>
+    <t>Marketing management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Organisational behaviour </t>
+  </si>
+  <si>
+    <t>Production and operations management</t>
+  </si>
+  <si>
+    <t>BR</t>
+  </si>
+  <si>
+    <t>FM</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>OB</t>
+  </si>
+  <si>
+    <t>MH</t>
+  </si>
+  <si>
+    <t>MK</t>
+  </si>
+  <si>
+    <t>PI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compensation management </t>
+  </si>
+  <si>
+    <t>Entrepreneurship development</t>
+  </si>
+  <si>
+    <t>Industrial marketing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Management of financial services </t>
+  </si>
+  <si>
+    <t>Management of training and development</t>
+  </si>
+  <si>
+    <t>Marketing communication stratergy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Portfolio management </t>
+  </si>
+  <si>
+    <t>Principles of insurance and banking</t>
+  </si>
+  <si>
+    <t>Project management</t>
+  </si>
+  <si>
+    <t>Service marketing</t>
+  </si>
+  <si>
+    <t>MR</t>
+  </si>
+  <si>
+    <t>SR</t>
+  </si>
+  <si>
+    <t>IA</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>PT</t>
+  </si>
+  <si>
+    <t>PJ</t>
+  </si>
+  <si>
+    <t>EP</t>
+  </si>
+  <si>
+    <t>IL</t>
+  </si>
+  <si>
+    <t>SG</t>
+  </si>
+  <si>
+    <t>SY</t>
+  </si>
+  <si>
+    <t>NG</t>
+  </si>
+  <si>
+    <t>International marketing</t>
+  </si>
+  <si>
+    <t>MF</t>
+  </si>
+  <si>
+    <t>MO</t>
+  </si>
+  <si>
+    <t>PB</t>
+  </si>
+  <si>
+    <t>Principles and practices of management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Business communication </t>
+  </si>
+  <si>
+    <t>Computer applications for business</t>
+  </si>
+  <si>
+    <t>CB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Financial accounting </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Financial reporting statement and analysis </t>
+  </si>
+  <si>
+    <t>Foreign exchange management</t>
+  </si>
+  <si>
+    <t>Human resource planning and development</t>
+  </si>
+  <si>
+    <t>Legal framework governing human relations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Management processes and organisational behaviour </t>
+  </si>
+  <si>
+    <t>Manpower development for technological change</t>
+  </si>
+  <si>
+    <t>Organisation change and intervention strategies</t>
+  </si>
+  <si>
+    <t>Sales and distribution management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Statistics and anaysis of decision making </t>
+  </si>
+  <si>
+    <t>Strategic management</t>
+  </si>
+  <si>
+    <t>Working capital management</t>
+  </si>
+  <si>
+    <t>PD</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>BN</t>
+  </si>
+  <si>
+    <t>FA</t>
+  </si>
+  <si>
+    <t>FS</t>
+  </si>
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>MQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Business environment </t>
+  </si>
+  <si>
+    <t>FX</t>
+  </si>
+  <si>
+    <t>MX</t>
+  </si>
+  <si>
+    <t>BL</t>
+  </si>
+  <si>
+    <t>LF</t>
+  </si>
+  <si>
+    <t>WC</t>
+  </si>
+  <si>
+    <t>OI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">International financial management </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Financial derivative </t>
+  </si>
+  <si>
+    <t>FT</t>
+  </si>
+  <si>
+    <t>MJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corporate finance </t>
+  </si>
+  <si>
+    <t>CR</t>
+  </si>
+  <si>
+    <t>Legal environment</t>
+  </si>
+  <si>
+    <t>LE</t>
+  </si>
+  <si>
     <t>Dynamics of machine</t>
   </si>
   <si>
@@ -894,16 +1236,7 @@
     <t>Production technology</t>
   </si>
   <si>
-    <t>FM</t>
-  </si>
-  <si>
-    <t>MO</t>
-  </si>
-  <si>
-    <t>MT</t>
-  </si>
-  <si>
-    <t>PT</t>
+    <t>Strength of materials</t>
   </si>
   <si>
     <t>SL</t>
@@ -912,54 +1245,51 @@
     <t>Steam generator and power</t>
   </si>
   <si>
-    <t>SG</t>
-  </si>
-  <si>
     <t>Computer aided design and manufacturing</t>
   </si>
   <si>
-    <t>CF</t>
-  </si>
-  <si>
     <t>Machine design</t>
   </si>
   <si>
     <t>Mechanical vibrations</t>
   </si>
   <si>
+    <t>MV</t>
+  </si>
+  <si>
     <t>Refrigeration and air conditioning</t>
   </si>
   <si>
+    <t>RC</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tribology </t>
   </si>
   <si>
+    <t>TY</t>
+  </si>
+  <si>
     <t>Operation research</t>
   </si>
   <si>
     <t>Tribology and mechanical vibration</t>
   </si>
   <si>
-    <t>MN</t>
-  </si>
-  <si>
-    <t>MV</t>
-  </si>
-  <si>
-    <t>RC</t>
-  </si>
-  <si>
-    <t>TY</t>
-  </si>
-  <si>
     <t>TV</t>
   </si>
   <si>
     <t>Advanced manufacturing tech</t>
   </si>
   <si>
+    <t>AF</t>
+  </si>
+  <si>
     <t xml:space="preserve">Automobile engineering </t>
   </si>
   <si>
+    <t>AG</t>
+  </si>
+  <si>
     <t>Maintainence engineeirng</t>
   </si>
   <si>
@@ -969,40 +1299,25 @@
     <t>Statistical quality control and reliability</t>
   </si>
   <si>
+    <t>SQ</t>
+  </si>
+  <si>
+    <t>Entrepreneurship</t>
+  </si>
+  <si>
     <t>Non conventional manufacturing</t>
   </si>
   <si>
     <t>Powerplant engineering</t>
   </si>
   <si>
-    <t>EP</t>
-  </si>
-  <si>
-    <t>AF</t>
-  </si>
-  <si>
-    <t>AG</t>
-  </si>
-  <si>
-    <t>MG</t>
-  </si>
-  <si>
-    <t>MR</t>
-  </si>
-  <si>
-    <t>SQ</t>
-  </si>
-  <si>
-    <t>NG</t>
-  </si>
-  <si>
-    <t>PI</t>
-  </si>
-  <si>
-    <t>Entrepreneurship</t>
-  </si>
-  <si>
-    <t>Strength of materials</t>
+    <t xml:space="preserve">Business legislation </t>
+  </si>
+  <si>
+    <t>Strategies and systems</t>
+  </si>
+  <si>
+    <t>Master in business administration</t>
   </si>
 </sst>
 </file>
@@ -1350,7 +1665,87 @@
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1693,10 +2088,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:L205"/>
+  <dimension ref="A2:L270"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H188" workbookViewId="0">
-      <selection activeCell="M192" sqref="M192"/>
+    <sheetView tabSelected="1" topLeftCell="G237" workbookViewId="0">
+      <selection activeCell="I238" sqref="I238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1938,6 +2333,12 @@
       <c r="K23" s="1"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>405</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>211</v>
+      </c>
       <c r="G24" t="s">
         <v>29</v>
       </c>
@@ -3008,584 +3409,1200 @@
     </row>
     <row r="139" spans="8:11" x14ac:dyDescent="0.25">
       <c r="I139" t="s">
+        <v>258</v>
+      </c>
+      <c r="J139" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="140" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="I140" t="s">
         <v>195</v>
       </c>
-      <c r="J139" t="s">
+      <c r="J140" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="140" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H140">
+    <row r="141" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H141">
         <v>6</v>
       </c>
-      <c r="I140" t="s">
+      <c r="I141" t="s">
         <v>197</v>
       </c>
-      <c r="J140" t="s">
+      <c r="J141" t="s">
         <v>198</v>
-      </c>
-    </row>
-    <row r="141" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="I141" t="s">
-        <v>92</v>
-      </c>
-      <c r="J141" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="142" spans="8:11" x14ac:dyDescent="0.25">
       <c r="I142" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J142" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="143" spans="8:11" x14ac:dyDescent="0.25">
       <c r="I143" t="s">
-        <v>199</v>
+        <v>94</v>
       </c>
       <c r="J143" t="s">
-        <v>200</v>
+        <v>99</v>
       </c>
     </row>
     <row r="144" spans="8:11" x14ac:dyDescent="0.25">
       <c r="I144" t="s">
-        <v>89</v>
+        <v>199</v>
       </c>
       <c r="J144" t="s">
-        <v>90</v>
+        <v>200</v>
       </c>
     </row>
     <row r="145" spans="8:10" x14ac:dyDescent="0.25">
       <c r="I145" t="s">
-        <v>201</v>
+        <v>89</v>
       </c>
       <c r="J145" t="s">
-        <v>202</v>
+        <v>90</v>
       </c>
     </row>
     <row r="146" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H146">
-        <v>7</v>
-      </c>
       <c r="I146" t="s">
-        <v>214</v>
+        <v>54</v>
       </c>
       <c r="J146" t="s">
-        <v>203</v>
+        <v>53</v>
       </c>
     </row>
     <row r="147" spans="8:10" x14ac:dyDescent="0.25">
       <c r="I147" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="J147" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="148" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H148">
+        <v>7</v>
+      </c>
       <c r="I148" t="s">
-        <v>60</v>
+        <v>214</v>
       </c>
       <c r="J148" t="s">
-        <v>61</v>
+        <v>203</v>
       </c>
     </row>
     <row r="149" spans="8:10" x14ac:dyDescent="0.25">
       <c r="I149" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="J149" t="s">
-        <v>21</v>
+        <v>205</v>
       </c>
     </row>
     <row r="150" spans="8:10" x14ac:dyDescent="0.25">
       <c r="I150" t="s">
-        <v>215</v>
+        <v>60</v>
       </c>
       <c r="J150" t="s">
-        <v>207</v>
+        <v>61</v>
       </c>
     </row>
     <row r="151" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H151">
-        <v>8</v>
-      </c>
       <c r="I151" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="J151" t="s">
-        <v>209</v>
+        <v>21</v>
       </c>
     </row>
     <row r="152" spans="8:10" x14ac:dyDescent="0.25">
       <c r="I152" t="s">
-        <v>64</v>
+        <v>260</v>
       </c>
       <c r="J152" t="s">
-        <v>65</v>
+        <v>261</v>
       </c>
     </row>
     <row r="153" spans="8:10" x14ac:dyDescent="0.25">
       <c r="I153" t="s">
-        <v>54</v>
+        <v>215</v>
       </c>
       <c r="J153" t="s">
-        <v>53</v>
+        <v>207</v>
       </c>
     </row>
     <row r="154" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H154">
+        <v>8</v>
+      </c>
       <c r="I154" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="J154" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="155" spans="8:10" x14ac:dyDescent="0.25">
       <c r="I155" t="s">
-        <v>185</v>
+        <v>64</v>
       </c>
       <c r="J155" t="s">
-        <v>189</v>
+        <v>65</v>
       </c>
     </row>
     <row r="156" spans="8:10" x14ac:dyDescent="0.25">
       <c r="I156" t="s">
-        <v>212</v>
+        <v>54</v>
       </c>
       <c r="J156" t="s">
-        <v>213</v>
+        <v>53</v>
       </c>
     </row>
     <row r="157" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H157" t="s">
-        <v>223</v>
+      <c r="I157" t="s">
+        <v>210</v>
+      </c>
+      <c r="J157" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="158" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H158">
-        <v>4</v>
-      </c>
       <c r="I158" t="s">
-        <v>257</v>
+        <v>185</v>
       </c>
       <c r="J158" t="s">
-        <v>224</v>
+        <v>189</v>
       </c>
     </row>
     <row r="159" spans="8:10" x14ac:dyDescent="0.25">
       <c r="I159" t="s">
-        <v>123</v>
+        <v>262</v>
       </c>
       <c r="J159" t="s">
-        <v>120</v>
+        <v>263</v>
       </c>
     </row>
     <row r="160" spans="8:10" x14ac:dyDescent="0.25">
       <c r="I160" t="s">
+        <v>264</v>
+      </c>
+      <c r="J160" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="161" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="I161" t="s">
+        <v>45</v>
+      </c>
+      <c r="J161" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="162" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="I162" t="s">
+        <v>66</v>
+      </c>
+      <c r="J162" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="163" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="I163" t="s">
+        <v>212</v>
+      </c>
+      <c r="J163" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="164" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H164" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="165" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H165">
+        <v>4</v>
+      </c>
+      <c r="I165" t="s">
+        <v>257</v>
+      </c>
+      <c r="J165" t="s">
+        <v>224</v>
+      </c>
+      <c r="K165">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="I166" t="s">
+        <v>123</v>
+      </c>
+      <c r="J166" t="s">
+        <v>120</v>
+      </c>
+      <c r="K166">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="167" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="I167" t="s">
         <v>225</v>
       </c>
-      <c r="J160" t="s">
+      <c r="J167" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="161" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="I161" t="s">
+      <c r="K167">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="168" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="I168" t="s">
         <v>227</v>
       </c>
-      <c r="J161" t="s">
+      <c r="J168" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="162" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="I162" t="s">
+      <c r="K168">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="169" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="I169" t="s">
         <v>157</v>
       </c>
-      <c r="J162" t="s">
+      <c r="J169" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="163" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="I163" t="s">
+      <c r="K169">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="170" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="I170" t="s">
         <v>249</v>
       </c>
-      <c r="J163" t="s">
+      <c r="J170" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="164" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="I164" t="s">
+      <c r="K170">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="171" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="I171" t="s">
         <v>229</v>
       </c>
-      <c r="J164" t="s">
+      <c r="J171" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="165" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H165">
+      <c r="K171">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="172" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H172">
         <v>6</v>
       </c>
-      <c r="I165" t="s">
+      <c r="I172" t="s">
         <v>231</v>
       </c>
-      <c r="J165" t="s">
+      <c r="J172" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="166" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="I166" t="s">
+      <c r="K172">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="I173" t="s">
         <v>169</v>
       </c>
-      <c r="J166" t="s">
+      <c r="J173" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="167" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="I167" t="s">
+      <c r="K173">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="174" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="I174" t="s">
         <v>233</v>
       </c>
-      <c r="J167" t="s">
+      <c r="J174" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="168" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="I168" t="s">
+      <c r="K174">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="175" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="I175" t="s">
         <v>251</v>
       </c>
-      <c r="J168" t="s">
+      <c r="J175" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="169" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="I169" t="s">
+      <c r="K175">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="176" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="I176" t="s">
         <v>159</v>
       </c>
-      <c r="J169" t="s">
+      <c r="J176" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="170" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="I170" t="s">
+      <c r="K176">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="177" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="I177" t="s">
         <v>235</v>
       </c>
-      <c r="J170" t="s">
+      <c r="J177" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="171" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="I171" t="s">
+      <c r="K177">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="178" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="I178" t="s">
         <v>237</v>
       </c>
-      <c r="J171" t="s">
+      <c r="J178" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="172" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H172">
+      <c r="K178">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="179" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H179">
         <v>7</v>
       </c>
-      <c r="I172" t="s">
+      <c r="I179" t="s">
         <v>239</v>
       </c>
-      <c r="J172" t="s">
+      <c r="J179" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="173" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="I173" t="s">
+      <c r="K179">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="I180" t="s">
         <v>241</v>
       </c>
-      <c r="J173" t="s">
+      <c r="J180" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="174" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="I174" t="s">
+      <c r="K180">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="181" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="I181" t="s">
         <v>253</v>
       </c>
-      <c r="J174" t="s">
+      <c r="J181" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="175" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="I175" t="s">
+      <c r="K181">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="182" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="I182" t="s">
         <v>160</v>
       </c>
-      <c r="J175" t="s">
+      <c r="J182" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="176" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="I176" t="s">
+      <c r="K182">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="183" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="I183" t="s">
         <v>243</v>
       </c>
-      <c r="J176" t="s">
+      <c r="J183" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="177" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H177">
+      <c r="K183">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="184" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H184">
         <v>8</v>
       </c>
-      <c r="I177" t="s">
+      <c r="I184" t="s">
         <v>245</v>
       </c>
-      <c r="J177" t="s">
+      <c r="J184" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="178" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="I178" t="s">
+      <c r="K184">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="I185" t="s">
         <v>105</v>
       </c>
-      <c r="J178" t="s">
+      <c r="J185" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="179" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="I179" t="s">
+      <c r="K185">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="186" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="I186" t="s">
         <v>247</v>
       </c>
-      <c r="J179" t="s">
+      <c r="J186" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="180" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="I180" t="s">
+      <c r="K186">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="187" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="I187" t="s">
         <v>255</v>
       </c>
-      <c r="J180" t="s">
+      <c r="J187" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="181" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H181" t="s">
+      <c r="K187">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="188" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H188" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="182" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H182">
+    <row r="189" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H189">
         <v>4</v>
       </c>
-      <c r="I182" t="s">
-        <v>258</v>
-      </c>
-      <c r="J182" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="183" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="I183" t="s">
-        <v>260</v>
-      </c>
-      <c r="J183" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="184" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="I184" t="s">
-        <v>261</v>
-      </c>
-      <c r="J184" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="185" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="I185" t="s">
-        <v>262</v>
-      </c>
-      <c r="J185" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="186" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="I186" t="s">
-        <v>263</v>
-      </c>
-      <c r="J186" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="187" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="I187" t="s">
-        <v>300</v>
-      </c>
-      <c r="J187" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="188" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="I188" t="s">
-        <v>269</v>
-      </c>
-      <c r="J188" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="189" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H189">
-        <v>6</v>
-      </c>
       <c r="I189" t="s">
-        <v>271</v>
+        <v>372</v>
       </c>
       <c r="J189" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="190" spans="8:10" x14ac:dyDescent="0.25">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="190" spans="8:11" x14ac:dyDescent="0.25">
       <c r="I190" t="s">
-        <v>273</v>
+        <v>374</v>
       </c>
       <c r="J190" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="191" spans="8:10" x14ac:dyDescent="0.25">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="191" spans="8:11" x14ac:dyDescent="0.25">
       <c r="I191" t="s">
-        <v>274</v>
+        <v>375</v>
       </c>
       <c r="J191" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="192" spans="8:10" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="192" spans="8:11" x14ac:dyDescent="0.25">
       <c r="I192" t="s">
-        <v>275</v>
+        <v>376</v>
       </c>
       <c r="J192" t="s">
-        <v>281</v>
+        <v>332</v>
       </c>
     </row>
     <row r="193" spans="8:10" x14ac:dyDescent="0.25">
       <c r="I193" t="s">
-        <v>276</v>
+        <v>377</v>
       </c>
       <c r="J193" t="s">
-        <v>282</v>
+        <v>323</v>
       </c>
     </row>
     <row r="194" spans="8:10" x14ac:dyDescent="0.25">
       <c r="I194" t="s">
-        <v>277</v>
+        <v>378</v>
       </c>
       <c r="J194" t="s">
-        <v>248</v>
+        <v>379</v>
       </c>
     </row>
     <row r="195" spans="8:10" x14ac:dyDescent="0.25">
       <c r="I195" t="s">
-        <v>278</v>
+        <v>380</v>
       </c>
       <c r="J195" t="s">
-        <v>283</v>
+        <v>327</v>
       </c>
     </row>
     <row r="196" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H196">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I196" t="s">
-        <v>284</v>
+        <v>381</v>
       </c>
       <c r="J196" t="s">
-        <v>292</v>
+        <v>275</v>
       </c>
     </row>
     <row r="197" spans="8:10" x14ac:dyDescent="0.25">
       <c r="I197" t="s">
-        <v>285</v>
+        <v>382</v>
       </c>
       <c r="J197" t="s">
-        <v>293</v>
+        <v>276</v>
       </c>
     </row>
     <row r="198" spans="8:10" x14ac:dyDescent="0.25">
       <c r="I198" t="s">
-        <v>286</v>
+        <v>383</v>
       </c>
       <c r="J198" t="s">
-        <v>294</v>
+        <v>384</v>
       </c>
     </row>
     <row r="199" spans="8:10" x14ac:dyDescent="0.25">
       <c r="I199" t="s">
-        <v>287</v>
+        <v>385</v>
       </c>
       <c r="J199" t="s">
-        <v>295</v>
+        <v>386</v>
       </c>
     </row>
     <row r="200" spans="8:10" x14ac:dyDescent="0.25">
       <c r="I200" t="s">
-        <v>288</v>
+        <v>387</v>
       </c>
       <c r="J200" t="s">
-        <v>296</v>
+        <v>388</v>
       </c>
     </row>
     <row r="201" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H201">
-        <v>8</v>
-      </c>
       <c r="I201" t="s">
-        <v>299</v>
+        <v>389</v>
       </c>
       <c r="J201" t="s">
-        <v>291</v>
+        <v>248</v>
       </c>
     </row>
     <row r="202" spans="8:10" x14ac:dyDescent="0.25">
       <c r="I202" t="s">
-        <v>199</v>
+        <v>390</v>
       </c>
       <c r="J202" t="s">
-        <v>200</v>
+        <v>391</v>
       </c>
     </row>
     <row r="203" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H203">
+        <v>7</v>
+      </c>
       <c r="I203" t="s">
-        <v>289</v>
+        <v>392</v>
       </c>
       <c r="J203" t="s">
-        <v>297</v>
+        <v>393</v>
       </c>
     </row>
     <row r="204" spans="8:10" x14ac:dyDescent="0.25">
       <c r="I204" t="s">
-        <v>277</v>
+        <v>394</v>
       </c>
       <c r="J204" t="s">
-        <v>248</v>
+        <v>395</v>
       </c>
     </row>
     <row r="205" spans="8:10" x14ac:dyDescent="0.25">
       <c r="I205" t="s">
+        <v>396</v>
+      </c>
+      <c r="J205" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="206" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I206" t="s">
+        <v>397</v>
+      </c>
+      <c r="J206" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="207" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I207" t="s">
+        <v>398</v>
+      </c>
+      <c r="J207" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="208" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H208">
+        <v>8</v>
+      </c>
+      <c r="I208" t="s">
+        <v>400</v>
+      </c>
+      <c r="J208" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="209" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I209" t="s">
+        <v>199</v>
+      </c>
+      <c r="J209" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="210" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I210" t="s">
+        <v>401</v>
+      </c>
+      <c r="J210" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="211" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I211" t="s">
+        <v>389</v>
+      </c>
+      <c r="J211" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="212" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I212" t="s">
+        <v>402</v>
+      </c>
+      <c r="J212" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="213" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I213" s="4" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="214" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H214" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="215" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H215">
+        <v>1</v>
+      </c>
+      <c r="I215" t="s">
+        <v>268</v>
+      </c>
+      <c r="J215" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="216" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I216" t="s">
+        <v>269</v>
+      </c>
+      <c r="J216" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="217" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I217" t="s">
+        <v>270</v>
+      </c>
+      <c r="J217" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="218" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I218" t="s">
+        <v>271</v>
+      </c>
+      <c r="J218" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="219" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I219" t="s">
+        <v>289</v>
+      </c>
+      <c r="J219" t="s">
         <v>290</v>
       </c>
-      <c r="J205" t="s">
+    </row>
+    <row r="220" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I220" t="s">
+        <v>286</v>
+      </c>
+      <c r="J220" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="221" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I221" t="s">
+        <v>272</v>
+      </c>
+      <c r="J221" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="222" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H222">
+        <v>2</v>
+      </c>
+      <c r="I222" t="s">
+        <v>279</v>
+      </c>
+      <c r="J222" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="223" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I223" t="s">
+        <v>280</v>
+      </c>
+      <c r="J223" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="224" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I224" t="s">
+        <v>281</v>
+      </c>
+      <c r="J224" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="225" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I225" t="s">
+        <v>284</v>
+      </c>
+      <c r="J225" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="226" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I226" t="s">
+        <v>285</v>
+      </c>
+      <c r="J226" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="227" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H227">
+        <v>3</v>
+      </c>
+      <c r="I227" t="s">
+        <v>288</v>
+      </c>
+      <c r="J227" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="228" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H228" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="229" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H229">
+        <v>1</v>
+      </c>
+      <c r="I229" t="s">
+        <v>334</v>
+      </c>
+      <c r="J229" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="230" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I230" t="s">
+        <v>335</v>
+      </c>
+      <c r="J230" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="231" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I231" t="s">
+        <v>281</v>
+      </c>
+      <c r="J231" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="232" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I232" t="s">
+        <v>336</v>
+      </c>
+      <c r="J232" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="233" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I233" t="s">
+        <v>338</v>
+      </c>
+      <c r="J233" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="234" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I234" t="s">
+        <v>339</v>
+      </c>
+      <c r="J234" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="235" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I235" t="s">
+        <v>343</v>
+      </c>
+      <c r="J235" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="236" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I236" t="s">
+        <v>347</v>
+      </c>
+      <c r="J236" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="237" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I237" t="s">
+        <v>269</v>
+      </c>
+      <c r="J237" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="238" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I238" t="s">
+        <v>357</v>
+      </c>
+      <c r="J238" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="239" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H239">
+        <v>2</v>
+      </c>
+      <c r="I239" t="s">
+        <v>295</v>
+      </c>
+      <c r="J239" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="240" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I240" t="s">
+        <v>296</v>
+      </c>
+      <c r="J240" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="241" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I241" t="s">
+        <v>297</v>
+      </c>
+      <c r="J241" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="242" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I242" t="s">
         <v>298</v>
+      </c>
+      <c r="J242" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="243" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I243" t="s">
+        <v>299</v>
+      </c>
+      <c r="J243" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="244" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I244" t="s">
+        <v>300</v>
+      </c>
+      <c r="J244" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="245" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I245" t="s">
+        <v>340</v>
+      </c>
+      <c r="J245" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="246" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I246" t="s">
+        <v>368</v>
+      </c>
+      <c r="J246" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="247" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I247" t="s">
+        <v>370</v>
+      </c>
+      <c r="J247" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="248" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I248" t="s">
+        <v>301</v>
+      </c>
+      <c r="J248" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="249" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H249">
+        <v>4</v>
+      </c>
+      <c r="I249" t="s">
+        <v>309</v>
+      </c>
+      <c r="J249" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="250" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I250" t="s">
+        <v>310</v>
+      </c>
+      <c r="J250" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="251" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I251" t="s">
+        <v>311</v>
+      </c>
+      <c r="J251" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="252" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I252" t="s">
+        <v>330</v>
+      </c>
+      <c r="J252" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="253" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I253" t="s">
+        <v>312</v>
+      </c>
+      <c r="J253" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="254" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I254" t="s">
+        <v>313</v>
+      </c>
+      <c r="J254" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="255" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I255" t="s">
+        <v>314</v>
+      </c>
+      <c r="J255" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="256" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I256" t="s">
+        <v>315</v>
+      </c>
+      <c r="J256" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="257" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I257" t="s">
+        <v>316</v>
+      </c>
+      <c r="J257" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="258" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I258" t="s">
+        <v>317</v>
+      </c>
+      <c r="J258" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="259" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I259" t="s">
+        <v>318</v>
+      </c>
+      <c r="J259" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="260" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I260" t="s">
+        <v>341</v>
+      </c>
+      <c r="J260" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="261" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I261" t="s">
+        <v>365</v>
+      </c>
+      <c r="J261" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="262" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I262" t="s">
+        <v>364</v>
+      </c>
+      <c r="J262" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="263" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I263" t="s">
+        <v>404</v>
+      </c>
+      <c r="J263" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="264" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H264">
+        <v>3</v>
+      </c>
+      <c r="I264" t="s">
+        <v>403</v>
+      </c>
+      <c r="J264" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="265" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I265" t="s">
+        <v>342</v>
+      </c>
+      <c r="J265" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="266" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I266" t="s">
+        <v>344</v>
+      </c>
+      <c r="J266" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="267" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I267" t="s">
+        <v>345</v>
+      </c>
+      <c r="J267" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="268" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I268" t="s">
+        <v>346</v>
+      </c>
+      <c r="J268" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="269" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I269" t="s">
+        <v>348</v>
+      </c>
+      <c r="J269" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="270" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I270" t="s">
+        <v>349</v>
+      </c>
+      <c r="J270" t="s">
+        <v>362</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="J19:J87">
-    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J88:J104">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J24:J105">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="9"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J24:J108 J110:J294">
+  <conditionalFormatting sqref="J24:J108 J110:J188 J213:J343">
+    <cfRule type="duplicateValues" dxfId="10" priority="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I24:I188 I214:I570">
+    <cfRule type="duplicateValues" dxfId="9" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J24:J188 J213:J530">
+    <cfRule type="duplicateValues" dxfId="8" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I215:J917">
+    <cfRule type="duplicateValues" dxfId="7" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I216:I238">
+    <cfRule type="duplicateValues" dxfId="6" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J189:J212">
     <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I24:I521">
+  <conditionalFormatting sqref="I189:I212">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J24:J481">
+  <conditionalFormatting sqref="J189:J212">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>